<commit_message>
Changes in multiple folder
</commit_message>
<xml_diff>
--- a/Vocabulary.xlsx
+++ b/Vocabulary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Self Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C337A8F2-D722-4345-BD8D-E264DFA3E200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630A7618-7DD4-4F83-B2D2-5EF33DD52CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,43 +25,142 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Siloed</t>
-  </si>
-  <si>
-    <t>(of a system, process, department, etc.) isolated from others.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adversities </t>
-  </si>
-  <si>
-    <t>a difficult or unpleasant situation</t>
-  </si>
-  <si>
-    <t>prone</t>
-  </si>
-  <si>
-    <t>likely or liable to suffer from, do, or experience something unpleasant or regrettable, lying flat, especially face downwards.</t>
-  </si>
-  <si>
-    <t>Ubiquitous</t>
-  </si>
-  <si>
-    <t>present, appearing, or found everywhere.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">articulate </t>
-  </si>
-  <si>
-    <t>having or showing the ability to speak fluently and coherently.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+  <si>
+    <t>Plunge</t>
+  </si>
+  <si>
+    <t>Varsity</t>
+  </si>
+  <si>
+    <t>relating to a university, विश्वविद्यालय</t>
+  </si>
+  <si>
+    <t>jump or dive quickly and energetically, डुबकी</t>
+  </si>
+  <si>
+    <t>Deterioration</t>
+  </si>
+  <si>
+    <t>the process of becoming progressively worse.</t>
+  </si>
+  <si>
+    <t>Mow</t>
+  </si>
+  <si>
+    <t>Cut down(grass) with machine</t>
+  </si>
+  <si>
+    <t>catastrophic</t>
+  </si>
+  <si>
+    <t>involving or causing sudden great damage or suffering.</t>
+  </si>
+  <si>
+    <t>ransom</t>
+  </si>
+  <si>
+    <t>a sum of money demanded or paid for the release of a captive.</t>
+  </si>
+  <si>
+    <t>captive</t>
+  </si>
+  <si>
+    <t>a person who has been taken prisoner or an animal that has been confined.</t>
+  </si>
+  <si>
+    <t>confined</t>
+  </si>
+  <si>
+    <t>(of a space) restricted in area or volume</t>
+  </si>
+  <si>
+    <t>eavesdrop</t>
+  </si>
+  <si>
+    <t>secretly listen to a conversation.</t>
+  </si>
+  <si>
+    <t>intrude</t>
+  </si>
+  <si>
+    <t>put oneself deliberately into a place or situation where one is unwelcome or uninvited.</t>
+  </si>
+  <si>
+    <t>make a physical attack on.</t>
+  </si>
+  <si>
+    <t>assault</t>
+  </si>
+  <si>
+    <t>gulity</t>
+  </si>
+  <si>
+    <t>अपराधी</t>
+  </si>
+  <si>
+    <t>prolonged</t>
+  </si>
+  <si>
+    <t>lengthy</t>
+  </si>
+  <si>
+    <t>consolidation</t>
+  </si>
+  <si>
+    <t>the action or process of combining a number of things into a single more effective or coherent whole.</t>
+  </si>
+  <si>
+    <t>furtive</t>
+  </si>
+  <si>
+    <t>attempting to avoid notice or attention, typically because of guilt or a belief that discovery would lead to trouble; secretive.</t>
+  </si>
+  <si>
+    <t>sneak</t>
+  </si>
+  <si>
+    <t>move or go in a furtive or stealthy way.</t>
+  </si>
+  <si>
+    <t>snoop</t>
+  </si>
+  <si>
+    <t>investigate or look around furtively in an attempt to find out something, especially information about someone's private affairs.</t>
+  </si>
+  <si>
+    <t>peculiar</t>
+  </si>
+  <si>
+    <t>different to what is normal or expected; strange.</t>
+  </si>
+  <si>
+    <t>ravel</t>
+  </si>
+  <si>
+    <t>opposite- tangle, unravel</t>
+  </si>
+  <si>
+    <t>untangle, entangle</t>
+  </si>
+  <si>
+    <t>stiletto</t>
+  </si>
+  <si>
+    <t>high heels</t>
+  </si>
+  <si>
+    <t>tranquility</t>
+  </si>
+  <si>
+    <t>calm, शांति</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,24 +170,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF2A3B4F"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF202124"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -113,18 +200,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,57 +493,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="113.1796875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="18.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="111.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.6328125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>